<commit_message>
Simulações com diferentes temperaturas
</commit_message>
<xml_diff>
--- a/output_transit_depth.xlsx
+++ b/output_transit_depth.xlsx
@@ -399,7 +399,7 @@
         <v>300.5</v>
       </c>
       <c r="C2">
-        <v>656.6310342721592</v>
+        <v>698.342243854011</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -410,7 +410,7 @@
         <v>314.5</v>
       </c>
       <c r="C3">
-        <v>554.3834728378716</v>
+        <v>593.6769593554159</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -421,7 +421,7 @@
         <v>328.4</v>
       </c>
       <c r="C4">
-        <v>554.2737198578341</v>
+        <v>593.0411156351845</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -432,7 +432,7 @@
         <v>342</v>
       </c>
       <c r="C5">
-        <v>626.0346221782509</v>
+        <v>666.4419341200212</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -443,7 +443,7 @@
         <v>356</v>
       </c>
       <c r="C6">
-        <v>624.95042417543</v>
+        <v>665.1522464695691</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -454,7 +454,7 @@
         <v>369.6</v>
       </c>
       <c r="C7">
-        <v>640.3493814850502</v>
+        <v>680.6202059079781</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -465,7 +465,7 @@
         <v>383.5</v>
       </c>
       <c r="C8">
-        <v>695.4750411678478</v>
+        <v>736.3712711970783</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -476,7 +476,7 @@
         <v>397.5</v>
       </c>
       <c r="C9">
-        <v>661.9225495763103</v>
+        <v>702.319849793187</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -487,7 +487,7 @@
         <v>411.1</v>
       </c>
       <c r="C10">
-        <v>647.9990654226775</v>
+        <v>688.2115340245409</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -498,7 +498,7 @@
         <v>425</v>
       </c>
       <c r="C11">
-        <v>678.0768024284845</v>
+        <v>718.6013598591279</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -509,7 +509,7 @@
         <v>439</v>
       </c>
       <c r="C12">
-        <v>680.7148198624269</v>
+        <v>721.1324989108148</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -520,7 +520,7 @@
         <v>452.6</v>
       </c>
       <c r="C13">
-        <v>668.6534341868721</v>
+        <v>708.8691411460957</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -531,7 +531,7 @@
         <v>466.6</v>
       </c>
       <c r="C14">
-        <v>674.5582942518924</v>
+        <v>714.8109949277615</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -542,7 +542,7 @@
         <v>480.5</v>
       </c>
       <c r="C15">
-        <v>678.298759601792</v>
+        <v>718.6004537045321</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -553,7 +553,7 @@
         <v>494.1</v>
       </c>
       <c r="C16">
-        <v>696.7963625196249</v>
+        <v>737.2757459551682</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -564,7 +564,7 @@
         <v>508.3</v>
       </c>
       <c r="C17">
-        <v>709.9960680821971</v>
+        <v>750.6694883916421</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -575,7 +575,7 @@
         <v>522</v>
       </c>
       <c r="C18">
-        <v>727.7304293279441</v>
+        <v>768.3922218387762</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -586,7 +586,7 @@
         <v>535.5999999999999</v>
       </c>
       <c r="C19">
-        <v>722.5783429246624</v>
+        <v>763.1498285415316</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -597,7 +597,7 @@
         <v>550</v>
       </c>
       <c r="C20">
-        <v>724.0325490375233</v>
+        <v>764.5814621501934</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -608,7 +608,7 @@
         <v>563.5</v>
       </c>
       <c r="C21">
-        <v>729.9840552875692</v>
+        <v>770.5334982478496</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -619,7 +619,7 @@
         <v>588.4000000000001</v>
       </c>
       <c r="C22">
-        <v>739.2722755696913</v>
+        <v>779.8273020018787</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -630,7 +630,7 @@
         <v>614</v>
       </c>
       <c r="C23">
-        <v>749.4004912241836</v>
+        <v>789.9509190403276</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -641,7 +641,7 @@
         <v>639</v>
       </c>
       <c r="C24">
-        <v>759.1525413327415</v>
+        <v>799.6833002618109</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -652,7 +652,7 @@
         <v>664.6</v>
       </c>
       <c r="C25">
-        <v>765.0527908709126</v>
+        <v>805.5469223620104</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -663,7 +663,7 @@
         <v>689.5</v>
       </c>
       <c r="C26">
-        <v>771.3462583190944</v>
+        <v>811.8072862606241</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -674,7 +674,7 @@
         <v>715</v>
       </c>
       <c r="C27">
-        <v>777.2554163424372</v>
+        <v>817.6684168161863</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -685,7 +685,7 @@
         <v>740</v>
       </c>
       <c r="C28">
-        <v>786.0317567379705</v>
+        <v>826.3841619271517</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -696,7 +696,7 @@
         <v>765</v>
       </c>
       <c r="C29">
-        <v>791.2119179973587</v>
+        <v>831.5088430658202</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -707,7 +707,7 @@
         <v>790.5</v>
       </c>
       <c r="C30">
-        <v>794.5813229389697</v>
+        <v>834.8227068875058</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -718,7 +718,7 @@
         <v>816</v>
       </c>
       <c r="C31">
-        <v>801.0297373062248</v>
+        <v>841.1974692998924</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -729,7 +729,7 @@
         <v>841.3000000000001</v>
       </c>
       <c r="C32">
-        <v>804.7532427156723</v>
+        <v>844.8471400407387</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -740,7 +740,7 @@
         <v>866</v>
       </c>
       <c r="C33">
-        <v>808.3557613749459</v>
+        <v>848.3788786642909</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -751,7 +751,7 @@
         <v>891.5999999999999</v>
       </c>
       <c r="C34">
-        <v>811.5521788139013</v>
+        <v>851.4976800779727</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -762,7 +762,7 @@
         <v>917</v>
       </c>
       <c r="C35">
-        <v>814.0400577695273</v>
+        <v>853.9148473436509</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -773,7 +773,7 @@
         <v>942.4</v>
       </c>
       <c r="C36">
-        <v>816.2662377425578</v>
+        <v>856.0605157041934</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -784,7 +784,7 @@
         <v>967.3000000000001</v>
       </c>
       <c r="C37">
-        <v>818.9181048419148</v>
+        <v>858.6283344400591</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -795,7 +795,7 @@
         <v>992.7</v>
       </c>
       <c r="C38">
-        <v>820.3558913222331</v>
+        <v>859.9942350322465</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -806,7 +806,7 @@
         <v>1018</v>
       </c>
       <c r="C39">
-        <v>822.4947884886146</v>
+        <v>862.0399480187002</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -817,7 +817,7 @@
         <v>1055</v>
       </c>
       <c r="C40">
-        <v>825.6635991585881</v>
+        <v>865.0750422755093</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -828,7 +828,7 @@
         <v>1083</v>
       </c>
       <c r="C41">
-        <v>828.1119404613956</v>
+        <v>867.4083611793782</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -839,7 +839,7 @@
         <v>1112</v>
       </c>
       <c r="C42">
-        <v>828.4245631856591</v>
+        <v>867.6301866678004</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -850,7 +850,7 @@
         <v>1143</v>
       </c>
       <c r="C43">
-        <v>830.2095209026251</v>
+        <v>869.2860803497515</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -861,7 +861,7 @@
         <v>1174</v>
       </c>
       <c r="C44">
-        <v>831.4478019559867</v>
+        <v>870.4101049136215</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -872,7 +872,7 @@
         <v>1205</v>
       </c>
       <c r="C45">
-        <v>832.5191975615543</v>
+        <v>871.3663389674498</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -883,7 +883,7 @@
         <v>1237</v>
       </c>
       <c r="C46">
-        <v>832.8385203089094</v>
+        <v>871.5631265351353</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -894,7 +894,7 @@
         <v>1271</v>
       </c>
       <c r="C47">
-        <v>833.6572875459192</v>
+        <v>872.2474665332492</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -905,7 +905,7 @@
         <v>1306</v>
       </c>
       <c r="C48">
-        <v>834.914545806753</v>
+        <v>873.3546947625737</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -916,7 +916,7 @@
         <v>1341</v>
       </c>
       <c r="C49">
-        <v>835.4956584563089</v>
+        <v>873.8045907060732</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -927,7 +927,7 @@
         <v>1377</v>
       </c>
       <c r="C50">
-        <v>836.9161561460058</v>
+        <v>875.0707375694278</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -938,7 +938,7 @@
         <v>1414</v>
       </c>
       <c r="C51">
-        <v>838.8917674043705</v>
+        <v>876.8854149621142</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -949,7 +949,7 @@
         <v>1452</v>
       </c>
       <c r="C52">
-        <v>841.0826576311647</v>
+        <v>878.911688527273</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -960,7 +960,7 @@
         <v>1492</v>
       </c>
       <c r="C53">
-        <v>844.969708357901</v>
+        <v>882.6043870351352</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -971,7 +971,7 @@
         <v>1532</v>
       </c>
       <c r="C54">
-        <v>848.6991714512504</v>
+        <v>886.1543106184478</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -982,7 +982,7 @@
         <v>1573</v>
       </c>
       <c r="C55">
-        <v>854.5857068447127</v>
+        <v>891.8155747982271</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -993,7 +993,7 @@
         <v>1616</v>
       </c>
       <c r="C56">
-        <v>860.2415293835763</v>
+        <v>897.2423174790079</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1004,7 +1004,7 @@
         <v>1659</v>
       </c>
       <c r="C57">
-        <v>862.7794304039149</v>
+        <v>899.5856096751797</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1015,7 +1015,7 @@
         <v>1704</v>
       </c>
       <c r="C58">
-        <v>863.8642467567737</v>
+        <v>900.4707647216615</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1026,7 +1026,7 @@
         <v>1751</v>
       </c>
       <c r="C59">
-        <v>865.1766039801112</v>
+        <v>901.5686295065217</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1037,7 +1037,7 @@
         <v>2098</v>
       </c>
       <c r="C60">
-        <v>869.6882321698185</v>
+        <v>904.656407209603</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1048,7 +1048,7 @@
         <v>2938</v>
       </c>
       <c r="C61">
-        <v>879.0786329866407</v>
+        <v>911.2034788496537</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1059,7 +1059,7 @@
         <v>3060</v>
       </c>
       <c r="C62">
-        <v>880.3908458218101</v>
+        <v>912.1673648400108</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1070,7 +1070,7 @@
         <v>3184</v>
       </c>
       <c r="C63">
-        <v>881.6740978919713</v>
+        <v>913.1174061474123</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1081,7 +1081,7 @@
         <v>3307</v>
       </c>
       <c r="C64">
-        <v>882.637016271448</v>
+        <v>913.7790811927226</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1092,7 +1092,7 @@
         <v>3430</v>
       </c>
       <c r="C65">
-        <v>883.747866377127</v>
+        <v>914.6378137127042</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Simulações para fator de impacto
</commit_message>
<xml_diff>
--- a/output_transit_depth.xlsx
+++ b/output_transit_depth.xlsx
@@ -377,7 +377,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -396,10 +396,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>417.7</v>
+        <v>300.5</v>
       </c>
       <c r="C2">
-        <v>363.6540506416486</v>
+        <v>704.3133693271919</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -407,10 +407,10 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>452.1</v>
+        <v>314.5</v>
       </c>
       <c r="C3">
-        <v>359.0745542395579</v>
+        <v>686.9740557409187</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -418,10 +418,10 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>486.8</v>
+        <v>328.4</v>
       </c>
       <c r="C4">
-        <v>354.961448346125</v>
+        <v>697.1478495955141</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -429,10 +429,10 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>521.5</v>
+        <v>342</v>
       </c>
       <c r="C5">
-        <v>350.2509029786882</v>
+        <v>708.8310419864907</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -440,10 +440,10 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>556</v>
+        <v>356</v>
       </c>
       <c r="C6">
-        <v>347.0411492597636</v>
+        <v>712.5912987658855</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -451,10 +451,10 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>563.5</v>
+        <v>369.6</v>
       </c>
       <c r="C7">
-        <v>346.1649692028113</v>
+        <v>718.2218431714959</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -462,10 +462,10 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>588.4000000000001</v>
+        <v>383.5</v>
       </c>
       <c r="C8">
-        <v>344.5837322092471</v>
+        <v>726.018359510916</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -473,10 +473,10 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>614</v>
+        <v>397.5</v>
       </c>
       <c r="C9">
-        <v>342.2496015912379</v>
+        <v>724.8644724312525</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -484,10 +484,10 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>639</v>
+        <v>411.1</v>
       </c>
       <c r="C10">
-        <v>340.3402613990636</v>
+        <v>722.577858361384</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -495,10 +495,10 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>664.6</v>
+        <v>425</v>
       </c>
       <c r="C11">
-        <v>338.1292137216718</v>
+        <v>727.0246601275287</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -506,10 +506,10 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>689.5</v>
+        <v>439</v>
       </c>
       <c r="C12">
-        <v>337.0536611088104</v>
+        <v>731.5756397161532</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -517,10 +517,10 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>715</v>
+        <v>452.6</v>
       </c>
       <c r="C13">
-        <v>335.2780991875415</v>
+        <v>731.7144591617586</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -528,10 +528,10 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>740</v>
+        <v>466.6</v>
       </c>
       <c r="C14">
-        <v>333.8077284642526</v>
+        <v>732.8499370130581</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -539,10 +539,10 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>765</v>
+        <v>480.5</v>
       </c>
       <c r="C15">
-        <v>332.4574394134583</v>
+        <v>732.0109699673338</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -550,10 +550,10 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>790.5</v>
+        <v>494.1</v>
       </c>
       <c r="C16">
-        <v>331.5046757255136</v>
+        <v>733.5484968087336</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -561,10 +561,10 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>816</v>
+        <v>508.3</v>
       </c>
       <c r="C17">
-        <v>330.3331087902706</v>
+        <v>730.5707453100218</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -572,10 +572,10 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>841.3000000000001</v>
+        <v>522</v>
       </c>
       <c r="C18">
-        <v>328.9271218186452</v>
+        <v>735.8716051000247</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -583,10 +583,10 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>866</v>
+        <v>535.5999999999999</v>
       </c>
       <c r="C19">
-        <v>327.6039502914107</v>
+        <v>737.6614333026721</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -594,10 +594,10 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>891.5999999999999</v>
+        <v>550</v>
       </c>
       <c r="C20">
-        <v>326.904147007423</v>
+        <v>738.4388434966693</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -605,10 +605,10 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>917</v>
+        <v>563.5</v>
       </c>
       <c r="C21">
-        <v>326.337685064515</v>
+        <v>739.7035098560823</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -616,10 +616,10 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>942.4</v>
+        <v>588.4000000000001</v>
       </c>
       <c r="C22">
-        <v>325.8595033246436</v>
+        <v>740.5995569664814</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -627,10 +627,10 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>967.3000000000001</v>
+        <v>614</v>
       </c>
       <c r="C23">
-        <v>325.1777759286645</v>
+        <v>741.3664004880527</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -638,10 +638,10 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>992.7</v>
+        <v>639</v>
       </c>
       <c r="C24">
-        <v>325.1445159363486</v>
+        <v>741.8630918425429</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -649,10 +649,10 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>1018</v>
+        <v>664.6</v>
       </c>
       <c r="C25">
-        <v>324.4560172231958</v>
+        <v>742.4857380700089</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -660,10 +660,10 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>1060</v>
+        <v>689.5</v>
       </c>
       <c r="C26">
-        <v>323.1848592670783</v>
+        <v>742.6864641844055</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -671,10 +671,10 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>1098</v>
+        <v>715</v>
       </c>
       <c r="C27">
-        <v>322.5507512440995</v>
+        <v>742.9212700500453</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -682,10 +682,10 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>1138</v>
+        <v>740</v>
       </c>
       <c r="C28">
-        <v>322.3701973158466</v>
+        <v>743.1444607878257</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -693,10 +693,10 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>1179</v>
+        <v>765</v>
       </c>
       <c r="C29">
-        <v>321.7804585626816</v>
+        <v>743.3359770652181</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -704,10 +704,10 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>1222</v>
+        <v>790.5</v>
       </c>
       <c r="C30">
-        <v>321.391865292342</v>
+        <v>743.5288691962638</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -715,10 +715,10 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>1266</v>
+        <v>816</v>
       </c>
       <c r="C31">
-        <v>320.8278465730574</v>
+        <v>743.5043738865943</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -726,10 +726,10 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>1312</v>
+        <v>841.3000000000001</v>
       </c>
       <c r="C32">
-        <v>320.4354453317792</v>
+        <v>743.5812612943682</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -737,10 +737,10 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>1358</v>
+        <v>866</v>
       </c>
       <c r="C33">
-        <v>319.8184799955151</v>
+        <v>743.6769156722312</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -748,10 +748,10 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>1408</v>
+        <v>891.5999999999999</v>
       </c>
       <c r="C34">
-        <v>318.5634300157947</v>
+        <v>743.7060042859711</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -759,10 +759,10 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>1459</v>
+        <v>917</v>
       </c>
       <c r="C35">
-        <v>317.5718713299691</v>
+        <v>743.7770749892936</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -770,10 +770,10 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>1512</v>
+        <v>942.4</v>
       </c>
       <c r="C36">
-        <v>316.0368097745447</v>
+        <v>743.8176213373504</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -781,10 +781,10 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>1566</v>
+        <v>967.3000000000001</v>
       </c>
       <c r="C37">
-        <v>314.4481552929124</v>
+        <v>743.7738191475862</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -792,10 +792,10 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>1623</v>
+        <v>992.7</v>
       </c>
       <c r="C38">
-        <v>312.9710084636139</v>
+        <v>743.7862621196833</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -803,10 +803,10 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>1682</v>
+        <v>1018</v>
       </c>
       <c r="C39">
-        <v>312.7663986918217</v>
+        <v>743.8876858174571</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -814,10 +814,285 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>1743</v>
+        <v>1055</v>
       </c>
       <c r="C40">
-        <v>311.813098995084</v>
+        <v>743.9433101416038</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="1">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>1083</v>
+      </c>
+      <c r="C41">
+        <v>744.1013491696901</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="1">
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <v>1112</v>
+      </c>
+      <c r="C42">
+        <v>744.132675177922</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="1">
+        <v>41</v>
+      </c>
+      <c r="B43">
+        <v>1143</v>
+      </c>
+      <c r="C43">
+        <v>744.243805770095</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="1">
+        <v>42</v>
+      </c>
+      <c r="B44">
+        <v>1174</v>
+      </c>
+      <c r="C44">
+        <v>744.3707989247539</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="1">
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <v>1205</v>
+      </c>
+      <c r="C45">
+        <v>744.56069659945</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="1">
+        <v>44</v>
+      </c>
+      <c r="B46">
+        <v>1237</v>
+      </c>
+      <c r="C46">
+        <v>744.7778539927397</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="1">
+        <v>45</v>
+      </c>
+      <c r="B47">
+        <v>1271</v>
+      </c>
+      <c r="C47">
+        <v>745.0123155428034</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+      <c r="B48">
+        <v>1306</v>
+      </c>
+      <c r="C48">
+        <v>745.3141678235297</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="B49">
+        <v>1341</v>
+      </c>
+      <c r="C49">
+        <v>745.7356408565596</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="1">
+        <v>48</v>
+      </c>
+      <c r="B50">
+        <v>1377</v>
+      </c>
+      <c r="C50">
+        <v>746.2094573807976</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="1">
+        <v>49</v>
+      </c>
+      <c r="B51">
+        <v>1414</v>
+      </c>
+      <c r="C51">
+        <v>746.7674708976357</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>1452</v>
+      </c>
+      <c r="C52">
+        <v>747.4083864059677</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="1">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>1492</v>
+      </c>
+      <c r="C53">
+        <v>747.927753055433</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="1">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <v>1532</v>
+      </c>
+      <c r="C54">
+        <v>748.4336959086013</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="1">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <v>1573</v>
+      </c>
+      <c r="C55">
+        <v>748.6162162658738</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="1">
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <v>1616</v>
+      </c>
+      <c r="C56">
+        <v>748.4099882123508</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="1">
+        <v>55</v>
+      </c>
+      <c r="B57">
+        <v>1659</v>
+      </c>
+      <c r="C57">
+        <v>748.1248621132863</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="1">
+        <v>56</v>
+      </c>
+      <c r="B58">
+        <v>1704</v>
+      </c>
+      <c r="C58">
+        <v>747.9217778639802</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="1">
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <v>1751</v>
+      </c>
+      <c r="C59">
+        <v>747.7542444689344</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="1">
+        <v>58</v>
+      </c>
+      <c r="B60">
+        <v>2098</v>
+      </c>
+      <c r="C60">
+        <v>746.2247628140517</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="1">
+        <v>59</v>
+      </c>
+      <c r="B61">
+        <v>2938</v>
+      </c>
+      <c r="C61">
+        <v>743.9612005673002</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="1">
+        <v>60</v>
+      </c>
+      <c r="B62">
+        <v>3060</v>
+      </c>
+      <c r="C62">
+        <v>743.7711936857384</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="1">
+        <v>61</v>
+      </c>
+      <c r="B63">
+        <v>3184</v>
+      </c>
+      <c r="C63">
+        <v>743.3964595170428</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="1">
+        <v>62</v>
+      </c>
+      <c r="B64">
+        <v>3307</v>
+      </c>
+      <c r="C64">
+        <v>743.2959976072517</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="1">
+        <v>63</v>
+      </c>
+      <c r="B65">
+        <v>3430</v>
+      </c>
+      <c r="C65">
+        <v>742.8183544393452</v>
       </c>
     </row>
   </sheetData>

</xml_diff>